<commit_message>
Final Random Forest Changes
</commit_message>
<xml_diff>
--- a/Random Forest Implementation/SensitivityVSPrecision.xlsx
+++ b/Random Forest Implementation/SensitivityVSPrecision.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Toxic</t>
   </si>
@@ -1852,6 +1852,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Tree Depth</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1917,6 +1972,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Precision</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3183,13 +3293,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>206060</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>9995</xdr:rowOff>
+      <xdr:rowOff>9994</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>279619</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>65447</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>165036</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3544,10 +3654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:I27"/>
+  <dimension ref="A5:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="101" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="101" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4029,6 +4139,54 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>